<commit_message>
Processus de traduction des éléments liés PN13 87a65c6ad52e47bfabd58c967042922b2620058b
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/CodeSystem-fr-note-scope-codes.xlsx
+++ b/VoitureBalaisDecisions/ig/CodeSystem-fr-note-scope-codes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-19T16:40:37+00:00</t>
+    <t>2025-08-20T14:11:18+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -190,12 +190,6 @@
   </si>
   <si>
     <t>Libellé textuel du médicament prescrit</t>
-  </si>
-  <si>
-    <t>LIPRESCPOS</t>
-  </si>
-  <si>
-    <t>Libellé textuel de la posologie</t>
   </si>
 </sst>
 </file>
@@ -506,7 +500,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -634,18 +628,6 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11">
-      <c r="A11" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>